<commit_message>
small adjustments for easy setup and first run
</commit_message>
<xml_diff>
--- a/final_data/final_data.xlsx
+++ b/final_data/final_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillhoffmann/Projects/uni/thesis/final_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillhoffmann/Projects/uni/kg-generation-for-educational-resources/final_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95AB11D-8F7A-1F4E-82AD-37DCE1A20A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F4948B-451F-434B-9B5E-37C9F221ABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21739,7 +21739,7 @@
   <dimension ref="A1:V477"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21836,7 +21836,9 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>22</v>
       </c>

</xml_diff>